<commit_message>
updated cod for ExcelDataRecorder for tree result
</commit_message>
<xml_diff>
--- a/src/main/resources/data_output/SequentialMemoryUsage.xlsx
+++ b/src/main/resources/data_output/SequentialMemoryUsage.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anul1 IS1.1 Semestrul2\MEvPerf\SearchAlgorithms\src\main\resources\data_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFCFA11-731D-4489-948A-D54350C35785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D8BC6B-50BA-4569-9D3D-90332EA5FD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Usage" sheetId="1" r:id="rId1"/>
@@ -20,25 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>BFS Memory Usage 10000 (bytes)</t>
-  </si>
-  <si>
-    <t>DFS Memory Usage 10000 (bytes)</t>
-  </si>
-  <si>
-    <t>BFS Memory Usage 1000 (bytes)</t>
-  </si>
-  <si>
-    <t>DFS Memory Usage 1000 (bytes)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Graph BFS Memory Usage 10000 (bytes)</t>
+  </si>
+  <si>
+    <t>Graph DFS Memory Usage 10000 (bytes)</t>
+  </si>
+  <si>
+    <t>Graph BFS Memory Usage 1000 (bytes)</t>
+  </si>
+  <si>
+    <t>Graph DFS Memory Usage 1000 (bytes)</t>
+  </si>
+  <si>
+    <t>Tree BFS Memory Usage 10000 (bytes)</t>
+  </si>
+  <si>
+    <t>Tree DFS Memory Usage 10000 (bytes)</t>
+  </si>
+  <si>
+    <t>Tree BFS Memory Usage 1000 (bytes)</t>
+  </si>
+  <si>
+    <t>Tree DFS Memory Usage 1000 (bytes)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,21 +395,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.44140625"/>
-    <col min="2" max="2" customWidth="true" width="30.21875"/>
-    <col min="3" max="3" customWidth="true" width="27.88671875"/>
-    <col min="4" max="4" customWidth="true" width="28.0"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="34.21875" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1"/>
+    <col min="5" max="6" width="33" customWidth="1"/>
+    <col min="7" max="7" width="31.77734375" customWidth="1"/>
+    <col min="8" max="8" width="32.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,143 +423,51 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>9411104</v>
+        <v>9312680</v>
       </c>
       <c r="B2">
-        <v>9185016</v>
+        <v>7982304</v>
       </c>
       <c r="C2">
-        <v>1331776</v>
+        <v>1316056</v>
       </c>
       <c r="D2">
-        <v>1331688</v>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>6658600</v>
+      </c>
+      <c r="F2">
+        <v>5326808</v>
+      </c>
+      <c r="G2">
+        <v>2663432</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>-5.57184E7</v>
-      </c>
-      <c r="B3" t="n">
-        <v>9111112.0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1312168.0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>9111176.0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>7809608.0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1328520.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>9321944.0</v>
-      </c>
-      <c r="B5" t="n">
-        <v>7990296.0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1301592.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1301568.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>7874784.0</v>
-      </c>
-      <c r="B6" t="n">
-        <v>9301696.0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1310128.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1310072.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>9321928.0</v>
-      </c>
-      <c r="B7" t="n">
-        <v>7990280.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1331688.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>9192224.0</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7879120.0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1298912.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" t="n">
-        <v>1331800.0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1331712.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" t="n">
-        <v>1331688.0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1331688.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" t="n">
-        <v>1331744.0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1331688.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" t="n">
-        <v>1331688.0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1331688.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" t="n">
-        <v>1300968.0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.0</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1316048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>